<commit_message>
update DORA for better rendering
remove ref_id for articles
</commit_message>
<xml_diff>
--- a/tools/dora/dora.xlsx
+++ b/tools/dora/dora.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/dora/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BF4421-B422-7046-A951-B1176CD6FBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19BA879-D714-1B42-BC06-9C797A8E0C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20480" xr2:uid="{07E11555-D7C4-E248-B1CA-88155D1FBDDE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20480" activeTab="1" xr2:uid="{07E11555-D7C4-E248-B1CA-88155D1FBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="2" r:id="rId1"/>
@@ -2282,8 +2282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE7C01F-A348-CC42-867E-C3FA7C84D7D7}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="241" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A13" zoomScale="241" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2428,8 +2428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B35FE3-E2E1-6544-BD94-781CE4F49196}">
   <dimension ref="A1:E304"/>
   <sheetViews>
-    <sheetView topLeftCell="A243" zoomScale="225" workbookViewId="0">
-      <selection activeCell="A300" sqref="A300"/>
+    <sheetView tabSelected="1" zoomScale="225" workbookViewId="0">
+      <selection activeCell="C297" sqref="C297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2484,9 +2484,7 @@
       <c r="B4" s="6">
         <v>3</v>
       </c>
-      <c r="C4" s="7">
-        <v>5</v>
-      </c>
+      <c r="C4" s="7"/>
       <c r="D4" s="6" t="s">
         <v>5</v>
       </c>
@@ -2761,9 +2759,7 @@
       <c r="B23" s="6">
         <v>3</v>
       </c>
-      <c r="C23" s="7">
-        <v>6</v>
-      </c>
+      <c r="C23" s="7"/>
       <c r="D23" s="6" t="s">
         <v>41</v>
       </c>
@@ -3046,9 +3042,7 @@
       <c r="B42" s="6">
         <v>3</v>
       </c>
-      <c r="C42" s="7">
-        <v>7</v>
-      </c>
+      <c r="C42" s="7"/>
       <c r="D42" s="6" t="s">
         <v>79</v>
       </c>
@@ -3134,9 +3128,7 @@
       <c r="B48" s="6">
         <v>3</v>
       </c>
-      <c r="C48" s="7">
-        <v>8</v>
-      </c>
+      <c r="C48" s="7"/>
       <c r="D48" s="6" t="s">
         <v>90</v>
       </c>
@@ -3254,9 +3246,7 @@
       <c r="B56" s="6">
         <v>3</v>
       </c>
-      <c r="C56" s="7">
-        <v>9</v>
-      </c>
+      <c r="C56" s="7"/>
       <c r="D56" s="6" t="s">
         <v>106</v>
       </c>
@@ -3505,9 +3495,7 @@
       <c r="B73" s="6">
         <v>3</v>
       </c>
-      <c r="C73" s="7">
-        <v>10</v>
-      </c>
+      <c r="C73" s="7"/>
       <c r="D73" s="6" t="s">
         <v>138</v>
       </c>
@@ -3593,9 +3581,7 @@
       <c r="B79" s="6">
         <v>3</v>
       </c>
-      <c r="C79" s="7">
-        <v>11</v>
-      </c>
+      <c r="C79" s="7"/>
       <c r="D79" s="6" t="s">
         <v>149</v>
       </c>
@@ -3887,9 +3873,7 @@
       <c r="B99" s="6">
         <v>3</v>
       </c>
-      <c r="C99" s="7">
-        <v>12</v>
-      </c>
+      <c r="C99" s="7"/>
       <c r="D99" s="6" t="s">
         <v>187</v>
       </c>
@@ -4119,9 +4103,7 @@
       <c r="B115" s="6">
         <v>3</v>
       </c>
-      <c r="C115" s="7">
-        <v>13</v>
-      </c>
+      <c r="C115" s="7"/>
       <c r="D115" s="6" t="s">
         <v>216</v>
       </c>
@@ -4310,9 +4292,7 @@
       <c r="B128" s="6">
         <v>3</v>
       </c>
-      <c r="C128" s="7">
-        <v>14</v>
-      </c>
+      <c r="C128" s="7"/>
       <c r="D128" s="6" t="s">
         <v>240</v>
       </c>
@@ -4370,9 +4350,7 @@
       <c r="B132" s="6">
         <v>3</v>
       </c>
-      <c r="C132" s="7">
-        <v>16</v>
-      </c>
+      <c r="C132" s="7"/>
       <c r="D132" s="6" t="s">
         <v>248</v>
       </c>
@@ -4568,9 +4546,7 @@
       <c r="B146" s="6">
         <v>2</v>
       </c>
-      <c r="C146" s="7">
-        <v>17</v>
-      </c>
+      <c r="C146" s="7"/>
       <c r="D146" s="7" t="s">
         <v>273</v>
       </c>
@@ -4718,9 +4694,7 @@
       <c r="B156" s="6">
         <v>2</v>
       </c>
-      <c r="C156" s="7">
-        <v>18</v>
-      </c>
+      <c r="C156" s="7"/>
       <c r="D156" s="6" t="s">
         <v>293</v>
       </c>
@@ -4853,9 +4827,7 @@
       <c r="B165" s="6">
         <v>2</v>
       </c>
-      <c r="C165" s="7">
-        <v>19</v>
-      </c>
+      <c r="C165" s="7"/>
       <c r="D165" s="7" t="s">
         <v>311</v>
       </c>
@@ -5088,9 +5060,7 @@
       <c r="B182" s="6">
         <v>2</v>
       </c>
-      <c r="C182" s="7">
-        <v>23</v>
-      </c>
+      <c r="C182" s="7"/>
       <c r="D182" s="7" t="s">
         <v>337</v>
       </c>
@@ -5129,9 +5099,7 @@
       <c r="B185" s="6">
         <v>2</v>
       </c>
-      <c r="C185" s="7">
-        <v>24</v>
-      </c>
+      <c r="C185" s="7"/>
       <c r="D185" s="7" t="s">
         <v>342</v>
       </c>
@@ -5236,9 +5204,7 @@
       <c r="B192" s="6">
         <v>2</v>
       </c>
-      <c r="C192" s="7">
-        <v>25</v>
-      </c>
+      <c r="C192" s="7"/>
       <c r="D192" s="7" t="s">
         <v>585</v>
       </c>
@@ -5296,9 +5262,7 @@
       <c r="B196" s="6">
         <v>2</v>
       </c>
-      <c r="C196" s="7">
-        <v>26</v>
-      </c>
+      <c r="C196" s="7"/>
       <c r="D196" s="7" t="s">
         <v>363</v>
       </c>
@@ -5509,9 +5473,7 @@
       <c r="B211" s="6">
         <v>2</v>
       </c>
-      <c r="C211" s="7">
-        <v>27</v>
-      </c>
+      <c r="C211" s="7"/>
       <c r="D211" s="7" t="s">
         <v>387</v>
       </c>
@@ -5715,9 +5677,7 @@
       <c r="B225" s="6">
         <v>3</v>
       </c>
-      <c r="C225" s="7">
-        <v>28</v>
-      </c>
+      <c r="C225" s="7"/>
       <c r="D225" s="7" t="s">
         <v>413</v>
       </c>
@@ -6201,9 +6161,7 @@
       <c r="B259" s="6">
         <v>3</v>
       </c>
-      <c r="C259" s="7">
-        <v>29</v>
-      </c>
+      <c r="C259" s="7"/>
       <c r="D259" s="7" t="s">
         <v>472</v>
       </c>
@@ -6333,9 +6291,7 @@
       <c r="B269" s="6">
         <v>3</v>
       </c>
-      <c r="C269" s="7">
-        <v>30</v>
-      </c>
+      <c r="C269" s="7"/>
       <c r="D269" s="7" t="s">
         <v>486</v>
       </c>
@@ -6745,9 +6701,7 @@
       <c r="B297" s="6">
         <v>2</v>
       </c>
-      <c r="C297" s="7">
-        <v>45</v>
-      </c>
+      <c r="C297" s="7"/>
       <c r="D297" s="5" t="s">
         <v>539</v>
       </c>

</xml_diff>

<commit_message>
make article 25 not assessable
</commit_message>
<xml_diff>
--- a/tools/dora/dora.xlsx
+++ b/tools/dora/dora.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/dora/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0A7E52-3471-CD41-9D46-87BF8EC9B407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C774BF-29FB-3741-B824-799AAAE90EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20480" activeTab="1" xr2:uid="{07E11555-D7C4-E248-B1CA-88155D1FBDDE}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1610" uniqueCount="1341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="1341">
   <si>
     <t>Depth</t>
   </si>
@@ -4588,7 +4588,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4928,7 +4928,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView zoomScale="241" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4952,7 +4952,7 @@
         <v>558</v>
       </c>
       <c r="B2" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -5073,8 +5073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B35FE3-E2E1-6544-BD94-781CE4F49196}">
   <dimension ref="A1:F699"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="176" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B397" sqref="B397"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10131,7 +10131,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A369" s="5" t="s">
         <v>555</v>
       </c>
@@ -10518,9 +10518,7 @@
       </c>
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A397" s="5" t="s">
-        <v>555</v>
-      </c>
+      <c r="A397" s="5"/>
       <c r="B397" s="7">
         <v>2</v>
       </c>
@@ -10825,7 +10823,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="419" spans="1:5" ht="195" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:5" ht="225" x14ac:dyDescent="0.2">
       <c r="A419" s="5"/>
       <c r="B419" s="7">
         <v>3</v>
@@ -12057,7 +12055,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="505" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="505" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A505" s="5" t="s">
         <v>555</v>
       </c>
@@ -12176,7 +12174,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="514" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="514" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A514" s="5"/>
       <c r="B514" s="7">
         <v>4</v>
@@ -12553,7 +12551,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="543" spans="1:5" ht="300" x14ac:dyDescent="0.2">
+    <row r="543" spans="1:5" ht="314" x14ac:dyDescent="0.2">
       <c r="A543" s="5"/>
       <c r="B543" s="7">
         <v>4</v>
@@ -13151,7 +13149,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="589" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+    <row r="589" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A589" s="5"/>
       <c r="B589" s="7">
         <v>4</v>
@@ -13759,7 +13757,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="635" spans="1:5" ht="117" x14ac:dyDescent="0.2">
+    <row r="635" spans="1:5" ht="130" x14ac:dyDescent="0.2">
       <c r="A635" s="5"/>
       <c r="B635" s="6">
         <v>3</v>
@@ -14262,7 +14260,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="674" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="674" spans="1:5" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A674" s="5"/>
       <c r="B674" s="6">
         <v>4</v>

</xml_diff>